<commit_message>
Antes da criação de novas tabelas
</commit_message>
<xml_diff>
--- a/AFazer.xlsx
+++ b/AFazer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ArgoMini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2278ABE-4DBC-4E63-A05C-928F4E6C4D4B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85E8B27-85B1-4A70-9263-8E65D2A68CA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{EC7DBF65-5471-4264-8307-EDACA57D583C}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>O usuário realizará a entrada de notas fiscais de compra</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Permitir inclusão de CPF no cupom fiscal.</t>
   </si>
   <si>
-    <t>Atualização de preços por atalho.</t>
-  </si>
-  <si>
     <t>Não será permitido a inclusão de produtos sem código de barras.</t>
   </si>
   <si>
@@ -113,13 +110,64 @@
   </si>
   <si>
     <t>horas que faço semanais</t>
+  </si>
+  <si>
+    <t>tela que recebe o codigo de barras</t>
+  </si>
+  <si>
+    <t>comunicação com o sefaz</t>
+  </si>
+  <si>
+    <t>busca da nota no sefaz</t>
+  </si>
+  <si>
+    <t>salva o xml</t>
+  </si>
+  <si>
+    <t>le o xml</t>
+  </si>
+  <si>
+    <t>processa o xml</t>
+  </si>
+  <si>
+    <t>da entrada na nota</t>
+  </si>
+  <si>
+    <t>salva estoque novo</t>
+  </si>
+  <si>
+    <t>cria produto q precisa criar</t>
+  </si>
+  <si>
+    <t>criar novo campo no frente de caixa</t>
+  </si>
+  <si>
+    <t>informar na nfe o cpf do cliente</t>
+  </si>
+  <si>
+    <t>criar novo campo em tela no frente caixa</t>
+  </si>
+  <si>
+    <t>le o xml e repete passos do codigo de barra</t>
+  </si>
+  <si>
+    <t>atualizar preco de custo</t>
+  </si>
+  <si>
+    <t>retirar item do cupom fiscal</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>sim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +177,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -170,6 +226,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,46 +541,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92959F33-21F8-44CA-9CC5-54B5EA9530D4}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="100.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>20</v>
+      <c r="B2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -531,43 +589,43 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>15</v>
       </c>
       <c r="D4" s="2">
         <f>D22/24</f>
-        <v>7.125</v>
+        <v>5.25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
       <c r="E5" s="5">
         <f>D22/6</f>
-        <v>28.5</v>
+        <v>21</v>
       </c>
       <c r="F5" s="5">
         <f>E5/7</f>
-        <v>4.0714285714285712</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -576,7 +634,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -584,7 +642,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -592,14 +650,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>12</v>
       </c>
       <c r="D8" s="3">
         <f>D22/22</f>
-        <v>7.7727272727272725</v>
+        <v>5.7272727272727275</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -607,35 +665,25 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="6">
-        <v>43398</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
-        <v>6</v>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -643,8 +691,8 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>6</v>
+      <c r="B12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,7 +721,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -683,8 +731,8 @@
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17">
-        <v>5</v>
+      <c r="B17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +770,135 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f>SUM(B2:B21)</f>
-        <v>171</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -744,19 +920,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H14" sqref="H14:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>